<commit_message>
get result real RF_GA
</commit_message>
<xml_diff>
--- a/rf_ga/10_07_classRF/結果グラフ.xlsx
+++ b/rf_ga/10_07_classRF/結果グラフ.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19470" windowHeight="15180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19476" windowHeight="15180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OOB" sheetId="8" r:id="rId1"/>
     <sheet name="Validation" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -41,19 +41,60 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>include</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>m</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>uniform</t>
+    <r>
+      <t>1+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>l</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +108,13 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,7 +161,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -179,6 +227,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -200,6 +251,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -220,6 +274,9 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-82CB-4782-A378-A0EA498416DD}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -247,6 +304,9 @@
                     </c:manualLayout>
                   </c15:layout>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -268,6 +328,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -287,6 +350,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="0"/>
@@ -374,23 +440,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>75.508550000000014</c:v>
+                  <c:v>79.458799999999982</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>84.444400000000002</c:v>
+                  <c:v>82.22199999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.943550000000002</c:v>
+                  <c:v>76.100500000000011</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.591000000000008</c:v>
+                  <c:v>75.070150000000012</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.748199999999997</c:v>
+                  <c:v>91.623800000000017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-82CB-4782-A378-A0EA498416DD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -428,6 +499,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -449,6 +523,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -470,6 +547,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -491,6 +571,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -511,6 +594,9 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-82CB-4782-A378-A0EA498416DD}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -599,23 +685,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>74.794300000000007</c:v>
+                  <c:v>77.370099999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.777699999999996</c:v>
+                  <c:v>81.666550000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.618149999999986</c:v>
+                  <c:v>75.516099999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75.709400000000016</c:v>
+                  <c:v>75.240950000000012</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.538500000000028</c:v>
+                  <c:v>91.367499999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-82CB-4782-A378-A0EA498416DD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -653,6 +744,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -674,6 +768,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -695,6 +792,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -716,6 +816,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -737,6 +840,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -756,6 +862,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-82CB-4782-A378-A0EA498416DD}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="0"/>
@@ -843,23 +952,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>75.952250000000006</c:v>
+                  <c:v>77.57565000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.222200000000001</c:v>
+                  <c:v>81.851800000000011</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.161799999999999</c:v>
+                  <c:v>75.58359999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>73.65055000000001</c:v>
+                  <c:v>75.06795000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90.730400000000017</c:v>
+                  <c:v>91.382900000000035</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-82CB-4782-A378-A0EA498416DD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
@@ -976,8 +1090,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="3.0213114712368299E-2"/>
-              <c:y val="0.35313774517007335"/>
+              <c:x val="1.9017329727944371E-2"/>
+              <c:y val="0.35313769167012016"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1123,7 +1237,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -1189,6 +1303,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1210,6 +1327,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1231,6 +1351,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1252,6 +1375,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1273,6 +1399,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1292,6 +1421,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="0"/>
@@ -1379,23 +1511,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>74.339750000000009</c:v>
+                  <c:v>77.835399999999993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>83.703649999999996</c:v>
+                  <c:v>80.555449999999979</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75.721900000000005</c:v>
+                  <c:v>76.364500000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74.946150000000003</c:v>
+                  <c:v>74.000749999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.359750000000005</c:v>
+                  <c:v>91.305249999999987</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-A92A-475D-B874-57DA907C2F72}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1433,6 +1570,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1454,6 +1594,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1475,6 +1618,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1496,6 +1642,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1516,6 +1665,9 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-A92A-475D-B874-57DA907C2F72}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1604,23 +1756,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>75.053999999999988</c:v>
+                  <c:v>78.755249999999975</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.036850000000001</c:v>
+                  <c:v>81.296149999999983</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75.265699999999995</c:v>
+                  <c:v>75.977399999999989</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74.76755</c:v>
+                  <c:v>73.524549999999991</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>90.87769999999999</c:v>
+                  <c:v>91.010050000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-A92A-475D-B874-57DA907C2F72}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1658,6 +1815,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1679,6 +1839,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1700,6 +1863,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1721,6 +1887,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1742,6 +1911,9 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                 </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1761,6 +1933,9 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-A92A-475D-B874-57DA907C2F72}"/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="#,##0.0_);[Red]\(#,##0.0\)" sourceLinked="0"/>
@@ -1848,23 +2023,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>77.153500000000008</c:v>
+                  <c:v>78.95004999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.222049999999996</c:v>
+                  <c:v>81.296149999999983</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75.008499999999984</c:v>
+                  <c:v>75.001750000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>74.831250000000011</c:v>
+                  <c:v>74.597400000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.507049999999992</c:v>
+                  <c:v>91.072149999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000013-A92A-475D-B874-57DA907C2F72}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
@@ -1981,8 +2161,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="3.0213114712368299E-2"/>
-              <c:y val="0.35313774517007335"/>
+              <c:x val="1.9017329727944371E-2"/>
+              <c:y val="0.35313769167012016"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3576,13 +3756,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:K22"/>
+    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3609,7 +3789,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3620,500 +3800,500 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
+        <v>0.95238</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.90476000000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.90476000000000001</v>
+      </c>
+      <c r="D3">
+        <v>0.81481000000000003</v>
+      </c>
+      <c r="E3">
+        <v>0.81481000000000003</v>
+      </c>
+      <c r="F3">
+        <v>0.81481000000000003</v>
+      </c>
+      <c r="G3">
+        <v>0.76315999999999995</v>
+      </c>
+      <c r="H3">
+        <v>0.73684000000000005</v>
+      </c>
+      <c r="I3">
+        <v>0.76315999999999995</v>
+      </c>
+      <c r="J3">
+        <v>0.73809999999999998</v>
+      </c>
+      <c r="K3">
+        <v>0.70238</v>
+      </c>
+      <c r="L3">
         <v>0.71428999999999998</v>
       </c>
-      <c r="B3" s="1">
+      <c r="M3">
+        <v>0.91601999999999995</v>
+      </c>
+      <c r="N3">
+        <v>0.91757</v>
+      </c>
+      <c r="O3">
+        <v>0.91446000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>0.81818000000000002</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.86363999999999996</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.81818000000000002</v>
+      </c>
+      <c r="D4">
+        <v>0.92593000000000003</v>
+      </c>
+      <c r="E4">
+        <v>0.92593000000000003</v>
+      </c>
+      <c r="F4">
+        <v>0.92593000000000003</v>
+      </c>
+      <c r="G4">
+        <v>0.67532000000000003</v>
+      </c>
+      <c r="H4">
         <v>0.71428999999999998</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.80952000000000002</v>
-      </c>
-      <c r="D3">
-        <v>0.92593000000000003</v>
-      </c>
-      <c r="E3">
-        <v>0.92593000000000003</v>
-      </c>
-      <c r="F3">
-        <v>0.85185</v>
-      </c>
-      <c r="G3">
-        <v>0.78947000000000001</v>
-      </c>
-      <c r="H3">
-        <v>0.76315999999999995</v>
-      </c>
-      <c r="I3">
-        <v>0.75</v>
-      </c>
-      <c r="J3">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="K3">
-        <v>0.79762</v>
-      </c>
-      <c r="L3">
-        <v>0.88095000000000001</v>
-      </c>
-      <c r="M3">
-        <v>0.92223999999999995</v>
-      </c>
-      <c r="N3">
-        <v>0.91913</v>
-      </c>
-      <c r="O3">
-        <v>0.91913</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
-        <v>0.68181999999999998</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.59091000000000005</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.86363999999999996</v>
-      </c>
-      <c r="D4">
-        <v>0.88888999999999996</v>
-      </c>
-      <c r="E4">
-        <v>0.85185</v>
-      </c>
-      <c r="F4">
-        <v>0.62963000000000002</v>
-      </c>
-      <c r="G4">
-        <v>0.74026000000000003</v>
-      </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.70130000000000003</v>
       </c>
-      <c r="I4">
-        <v>0.75324999999999998</v>
-      </c>
       <c r="J4">
-        <v>0.77646999999999999</v>
+        <v>0.72941</v>
       </c>
       <c r="K4">
         <v>0.74117999999999995</v>
       </c>
       <c r="L4">
-        <v>0.69411999999999996</v>
+        <v>0.70587999999999995</v>
       </c>
       <c r="M4">
-        <v>0.93167999999999995</v>
+        <v>0.92081000000000002</v>
       </c>
       <c r="N4">
-        <v>0.92701999999999996</v>
+        <v>0.91615000000000002</v>
       </c>
       <c r="O4">
-        <v>0.90061999999999998</v>
+        <v>0.92547000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>0.72726999999999997</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="B5" s="1">
-        <v>0.77273000000000003</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="C5" s="1">
-        <v>0.77273000000000003</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="D5">
-        <v>0.81481000000000003</v>
+        <v>0.88888999999999996</v>
       </c>
       <c r="E5">
-        <v>0.77778000000000003</v>
+        <v>0.88888999999999996</v>
       </c>
       <c r="F5">
-        <v>0.77778000000000003</v>
+        <v>0.88888999999999996</v>
       </c>
       <c r="G5">
         <v>0.72726999999999997</v>
       </c>
       <c r="H5">
-        <v>0.74026000000000003</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="I5">
-        <v>0.70130000000000003</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="J5">
-        <v>0.8</v>
+        <v>0.71765000000000001</v>
       </c>
       <c r="K5">
-        <v>0.8</v>
+        <v>0.69411999999999996</v>
       </c>
       <c r="L5">
         <v>0.74117999999999995</v>
       </c>
       <c r="M5">
-        <v>0.90993999999999997</v>
+        <v>0.91925000000000001</v>
       </c>
       <c r="N5">
-        <v>0.91303999999999996</v>
+        <v>0.92235999999999996</v>
       </c>
       <c r="O5">
-        <v>0.89751999999999998</v>
+        <v>0.91925000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>0.63636000000000004</v>
+        <v>0.77273000000000003</v>
       </c>
       <c r="B6" s="1">
-        <v>0.63636000000000004</v>
+        <v>0.77273000000000003</v>
       </c>
       <c r="C6" s="1">
         <v>0.81818000000000002</v>
       </c>
       <c r="D6">
-        <v>0.88888999999999996</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="E6">
-        <v>0.85185</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="F6">
-        <v>0.85185</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="G6">
-        <v>0.72726999999999997</v>
+        <v>0.79220999999999997</v>
       </c>
       <c r="H6">
-        <v>0.66234000000000004</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="I6">
-        <v>0.64934999999999998</v>
+        <v>0.77922000000000002</v>
       </c>
       <c r="J6">
-        <v>0.70587999999999995</v>
+        <v>0.76471</v>
       </c>
       <c r="K6">
-        <v>0.69411999999999996</v>
+        <v>0.76471</v>
       </c>
       <c r="L6">
-        <v>0.75294000000000005</v>
+        <v>0.77646999999999999</v>
       </c>
       <c r="M6">
-        <v>0.91303999999999996</v>
+        <v>0.89129999999999998</v>
       </c>
       <c r="N6">
-        <v>0.90683000000000002</v>
+        <v>0.89441000000000004</v>
       </c>
       <c r="O6">
-        <v>0.90527999999999997</v>
+        <v>0.88975000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>0.72726999999999997</v>
+        <v>0.59091000000000005</v>
       </c>
       <c r="B7" s="1">
-        <v>0.77273000000000003</v>
+        <v>0.45455000000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>0.63636000000000004</v>
+        <v>0.54544999999999999</v>
       </c>
       <c r="D7">
         <v>0.81481000000000003</v>
       </c>
       <c r="E7">
+        <v>0.77778000000000003</v>
+      </c>
+      <c r="F7">
         <v>0.81481000000000003</v>
       </c>
-      <c r="F7">
-        <v>0.88888999999999996</v>
-      </c>
       <c r="G7">
-        <v>0.75324999999999998</v>
+        <v>0.76622999999999997</v>
       </c>
       <c r="H7">
-        <v>0.81818000000000002</v>
+        <v>0.77922000000000002</v>
       </c>
       <c r="I7">
-        <v>0.77922000000000002</v>
+        <v>0.76622999999999997</v>
       </c>
       <c r="J7">
-        <v>0.71765000000000001</v>
+        <v>0.69411999999999996</v>
       </c>
       <c r="K7">
+        <v>0.67059000000000002</v>
+      </c>
+      <c r="L7">
+        <v>0.67059000000000002</v>
+      </c>
+      <c r="M7">
+        <v>0.91459999999999997</v>
+      </c>
+      <c r="N7">
+        <v>0.90839000000000003</v>
+      </c>
+      <c r="O7">
+        <v>0.91459999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>0.80952000000000002</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.80952000000000002</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.80952000000000002</v>
+      </c>
+      <c r="D8">
+        <v>0.81481000000000003</v>
+      </c>
+      <c r="E8">
+        <v>0.81481000000000003</v>
+      </c>
+      <c r="F8">
+        <v>0.77778000000000003</v>
+      </c>
+      <c r="G8">
+        <v>0.84416000000000002</v>
+      </c>
+      <c r="H8">
+        <v>0.79220999999999997</v>
+      </c>
+      <c r="I8">
+        <v>0.80518999999999996</v>
+      </c>
+      <c r="J8">
+        <v>0.75294000000000005</v>
+      </c>
+      <c r="K8">
+        <v>0.76471</v>
+      </c>
+      <c r="L8">
         <v>0.72941</v>
-      </c>
-      <c r="L7">
-        <v>0.69411999999999996</v>
-      </c>
-      <c r="M7">
-        <v>0.90839000000000003</v>
-      </c>
-      <c r="N7">
-        <v>0.90373000000000003</v>
-      </c>
-      <c r="O7">
-        <v>0.91303999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A8" s="1">
-        <v>0.66666999999999998</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.71428999999999998</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="D8">
-        <v>0.88888999999999996</v>
-      </c>
-      <c r="E8">
-        <v>0.85185</v>
-      </c>
-      <c r="F8">
-        <v>0.81481000000000003</v>
-      </c>
-      <c r="G8">
-        <v>0.75324999999999998</v>
-      </c>
-      <c r="H8">
-        <v>0.68830999999999998</v>
-      </c>
-      <c r="I8">
-        <v>0.71428999999999998</v>
-      </c>
-      <c r="J8">
-        <v>0.76471</v>
-      </c>
-      <c r="K8">
-        <v>0.74117999999999995</v>
-      </c>
-      <c r="L8">
-        <v>0.68235000000000001</v>
       </c>
       <c r="M8">
         <v>0.92701999999999996</v>
       </c>
       <c r="N8">
-        <v>0.91925000000000001</v>
+        <v>0.92391000000000001</v>
       </c>
       <c r="O8">
-        <v>0.92081000000000002</v>
+        <v>0.92857000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
+        <v>0.95238</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.85714000000000001</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.95238</v>
+      </c>
+      <c r="D9">
+        <v>0.77778000000000003</v>
+      </c>
+      <c r="E9">
+        <v>0.77778000000000003</v>
+      </c>
+      <c r="F9">
+        <v>0.77778000000000003</v>
+      </c>
+      <c r="G9">
+        <v>0.75324999999999998</v>
+      </c>
+      <c r="H9">
+        <v>0.75324999999999998</v>
+      </c>
+      <c r="I9">
+        <v>0.70130000000000003</v>
+      </c>
+      <c r="J9">
+        <v>0.71765000000000001</v>
+      </c>
+      <c r="K9">
+        <v>0.75294000000000005</v>
+      </c>
+      <c r="L9">
+        <v>0.74117999999999995</v>
+      </c>
+      <c r="M9">
+        <v>0.91601999999999995</v>
+      </c>
+      <c r="N9">
+        <v>0.91446000000000005</v>
+      </c>
+      <c r="O9">
+        <v>0.91601999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>0.80952000000000002</v>
       </c>
-      <c r="B9" s="1">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="B10" s="1">
         <v>0.80952000000000002</v>
-      </c>
-      <c r="D9">
-        <v>0.96296000000000004</v>
-      </c>
-      <c r="E9">
-        <v>0.92593000000000003</v>
-      </c>
-      <c r="F9">
-        <v>0.92593000000000003</v>
-      </c>
-      <c r="G9">
-        <v>0.79220999999999997</v>
-      </c>
-      <c r="H9">
-        <v>0.79220999999999997</v>
-      </c>
-      <c r="I9">
-        <v>0.80518999999999996</v>
-      </c>
-      <c r="J9">
-        <v>0.74117999999999995</v>
-      </c>
-      <c r="K9">
-        <v>0.81176000000000004</v>
-      </c>
-      <c r="L9">
-        <v>0.72941</v>
-      </c>
-      <c r="M9">
-        <v>0.91446000000000005</v>
-      </c>
-      <c r="N9">
-        <v>0.91134999999999999</v>
-      </c>
-      <c r="O9">
-        <v>0.90358000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A10" s="1">
-        <v>0.66666999999999998</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.61904999999999999</v>
       </c>
       <c r="C10" s="1">
         <v>0.76190000000000002</v>
       </c>
       <c r="D10">
-        <v>0.77778000000000003</v>
+        <v>0.85185</v>
       </c>
       <c r="E10">
-        <v>0.74073999999999995</v>
+        <v>0.85185</v>
       </c>
       <c r="F10">
-        <v>0.88888999999999996</v>
+        <v>0.85185</v>
       </c>
       <c r="G10">
-        <v>0.74026000000000003</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="H10">
-        <v>0.75324999999999998</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="I10">
-        <v>0.74026000000000003</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="J10">
-        <v>0.75</v>
+        <v>0.80952000000000002</v>
       </c>
       <c r="K10">
-        <v>0.73809999999999998</v>
+        <v>0.78571000000000002</v>
       </c>
       <c r="L10">
         <v>0.78571000000000002</v>
       </c>
       <c r="M10">
-        <v>0.93001999999999996</v>
+        <v>0.92223999999999995</v>
       </c>
       <c r="N10">
-        <v>0.93313000000000001</v>
+        <v>0.92535000000000001</v>
       </c>
       <c r="O10">
-        <v>0.89890999999999999</v>
+        <v>0.91757</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>0.66666999999999998</v>
+        <v>0.85714000000000001</v>
       </c>
       <c r="B11" s="1">
-        <v>0.57142999999999999</v>
+        <v>0.85714000000000001</v>
       </c>
       <c r="C11" s="1">
-        <v>0.66666999999999998</v>
+        <v>0.85714000000000001</v>
       </c>
       <c r="D11">
         <v>0.74073999999999995</v>
       </c>
       <c r="E11">
+        <v>0.85185</v>
+      </c>
+      <c r="F11">
         <v>0.74073999999999995</v>
       </c>
-      <c r="F11">
-        <v>0.77778000000000003</v>
-      </c>
       <c r="G11">
-        <v>0.76622999999999997</v>
+        <v>0.74026000000000003</v>
       </c>
       <c r="H11">
-        <v>0.75324999999999998</v>
+        <v>0.71428999999999998</v>
       </c>
       <c r="I11">
-        <v>0.75324999999999998</v>
+        <v>0.71428999999999998</v>
       </c>
       <c r="J11">
-        <v>0.78571000000000002</v>
+        <v>0.82142999999999999</v>
       </c>
       <c r="K11">
-        <v>0.77381</v>
+        <v>0.80952000000000002</v>
       </c>
       <c r="L11">
+        <v>0.83333000000000002</v>
+      </c>
+      <c r="M11">
+        <v>0.91757</v>
+      </c>
+      <c r="N11">
+        <v>0.91134999999999999</v>
+      </c>
+      <c r="O11">
+        <v>0.91601999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>0.61904999999999999</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.52381</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.57142999999999999</v>
+      </c>
+      <c r="D12">
+        <v>0.92593000000000003</v>
+      </c>
+      <c r="E12">
+        <v>0.85185</v>
+      </c>
+      <c r="F12">
+        <v>0.96296000000000004</v>
+      </c>
+      <c r="G12">
+        <v>0.76315999999999995</v>
+      </c>
+      <c r="H12">
         <v>0.75</v>
       </c>
-      <c r="M11">
-        <v>0.92068000000000005</v>
-      </c>
-      <c r="N11">
-        <v>0.91601999999999995</v>
-      </c>
-      <c r="O11">
-        <v>0.91291</v>
+      <c r="I12">
+        <v>0.78947000000000001</v>
+      </c>
+      <c r="J12">
+        <v>0.82142999999999999</v>
+      </c>
+      <c r="K12">
+        <v>0.80952000000000002</v>
+      </c>
+      <c r="L12">
+        <v>0.79762</v>
+      </c>
+      <c r="M12">
+        <v>0.90824000000000005</v>
+      </c>
+      <c r="N12">
+        <v>0.90046999999999999</v>
+      </c>
+      <c r="O12">
+        <v>0.89890999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A12" s="1">
-        <v>0.85714000000000001</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.90476000000000001</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0.71428999999999998</v>
-      </c>
-      <c r="D12">
-        <v>0.74073999999999995</v>
-      </c>
-      <c r="E12">
-        <v>0.74073999999999995</v>
-      </c>
-      <c r="F12">
-        <v>0.88888999999999996</v>
-      </c>
-      <c r="G12">
-        <v>0.78947000000000001</v>
-      </c>
-      <c r="H12">
-        <v>0.80262999999999995</v>
-      </c>
-      <c r="I12">
-        <v>0.80262999999999995</v>
-      </c>
-      <c r="J12">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="K12">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="L12">
-        <v>0.72619</v>
-      </c>
-      <c r="M12">
-        <v>0.90512999999999999</v>
-      </c>
-      <c r="N12">
-        <v>0.90824000000000005</v>
-      </c>
-      <c r="O12">
-        <v>0.91446000000000005</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0.80952000000000002</v>
       </c>
       <c r="B13" s="1">
-        <v>0.80952000000000002</v>
+        <v>0.76190000000000002</v>
       </c>
       <c r="C13" s="1">
-        <v>0.80952000000000002</v>
+        <v>0.71428999999999998</v>
       </c>
       <c r="D13">
-        <v>0.88888999999999996</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="E13">
-        <v>0.85185</v>
+        <v>0.77778000000000003</v>
       </c>
       <c r="F13">
-        <v>0.74073999999999995</v>
+        <v>0.77778000000000003</v>
       </c>
       <c r="G13">
-        <v>0.75</v>
+        <v>0.72367999999999999</v>
       </c>
       <c r="H13">
-        <v>0.76315999999999995</v>
+        <v>0.73684000000000005</v>
       </c>
       <c r="I13">
         <v>0.73684000000000005</v>
@@ -4122,406 +4302,406 @@
         <v>0.71428999999999998</v>
       </c>
       <c r="K13">
-        <v>0.70238</v>
+        <v>0.71428999999999998</v>
       </c>
       <c r="L13">
-        <v>0.75</v>
+        <v>0.71428999999999998</v>
       </c>
       <c r="M13">
-        <v>0.93467999999999996</v>
+        <v>0.92379</v>
       </c>
       <c r="N13">
-        <v>0.93157000000000001</v>
+        <v>0.92223999999999995</v>
       </c>
       <c r="O13">
-        <v>0.90512999999999999</v>
+        <v>0.92068000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>0.81818000000000002</v>
+        <v>0.86363999999999996</v>
       </c>
       <c r="B14" s="1">
-        <v>0.81818000000000002</v>
+        <v>0.86363999999999996</v>
       </c>
       <c r="C14" s="1">
-        <v>0.63636000000000004</v>
+        <v>0.86363999999999996</v>
       </c>
       <c r="D14">
         <v>0.77778000000000003</v>
       </c>
       <c r="E14">
-        <v>0.81481000000000003</v>
+        <v>0.74073999999999995</v>
       </c>
       <c r="F14">
         <v>0.85185</v>
       </c>
       <c r="G14">
-        <v>0.72726999999999997</v>
+        <v>0.77922000000000002</v>
       </c>
       <c r="H14">
-        <v>0.67532000000000003</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="I14">
-        <v>0.68830999999999998</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="J14">
         <v>0.71765000000000001</v>
       </c>
       <c r="K14">
-        <v>0.70587999999999995</v>
+        <v>0.77646999999999999</v>
       </c>
       <c r="L14">
-        <v>0.69411999999999996</v>
+        <v>0.72941</v>
       </c>
       <c r="M14">
-        <v>0.92081000000000002</v>
+        <v>0.92701999999999996</v>
       </c>
       <c r="N14">
-        <v>0.91769999999999996</v>
+        <v>0.92391000000000001</v>
       </c>
       <c r="O14">
-        <v>0.89751999999999998</v>
+        <v>0.92391000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>0.72726999999999997</v>
+        <v>0.90908999999999995</v>
       </c>
       <c r="B15" s="1">
         <v>0.77273000000000003</v>
       </c>
       <c r="C15" s="1">
-        <v>0.72726999999999997</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="D15">
+        <v>0.81481000000000003</v>
+      </c>
+      <c r="E15">
         <v>0.85185</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>0.77778000000000003</v>
       </c>
-      <c r="F15">
-        <v>0.74073999999999995</v>
-      </c>
       <c r="G15">
-        <v>0.74026000000000003</v>
+        <v>0.76622999999999997</v>
       </c>
       <c r="H15">
-        <v>0.74026000000000003</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="I15">
-        <v>0.76622999999999997</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="J15">
-        <v>0.74117999999999995</v>
+        <v>0.77646999999999999</v>
       </c>
       <c r="K15">
         <v>0.76471</v>
       </c>
       <c r="L15">
-        <v>0.71765000000000001</v>
+        <v>0.74117999999999995</v>
       </c>
       <c r="M15">
-        <v>0.93167999999999995</v>
+        <v>0.91615000000000002</v>
       </c>
       <c r="N15">
-        <v>0.92857000000000001</v>
+        <v>0.89907000000000004</v>
       </c>
       <c r="O15">
-        <v>0.88819999999999999</v>
+        <v>0.90839000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>0.86363999999999996</v>
+        <v>0.72726999999999997</v>
       </c>
       <c r="B16" s="1">
+        <v>0.72726999999999997</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.72726999999999997</v>
+      </c>
+      <c r="D16">
+        <v>0.81481000000000003</v>
+      </c>
+      <c r="E16">
+        <v>0.81481000000000003</v>
+      </c>
+      <c r="F16">
+        <v>0.77778000000000003</v>
+      </c>
+      <c r="G16">
+        <v>0.79220999999999997</v>
+      </c>
+      <c r="H16">
+        <v>0.74026000000000003</v>
+      </c>
+      <c r="I16">
+        <v>0.75324999999999998</v>
+      </c>
+      <c r="J16">
+        <v>0.78824000000000005</v>
+      </c>
+      <c r="K16">
+        <v>0.8</v>
+      </c>
+      <c r="L16">
+        <v>0.77646999999999999</v>
+      </c>
+      <c r="M16">
+        <v>0.91925000000000001</v>
+      </c>
+      <c r="N16">
+        <v>0.91925000000000001</v>
+      </c>
+      <c r="O16">
+        <v>0.91769999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>0.77273000000000003</v>
       </c>
-      <c r="C16" s="1">
-        <v>0.81818000000000002</v>
-      </c>
-      <c r="D16">
-        <v>0.88888999999999996</v>
-      </c>
-      <c r="E16">
-        <v>0.88888999999999996</v>
-      </c>
-      <c r="F16">
+      <c r="B17" s="1">
+        <v>0.77273000000000003</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.77273000000000003</v>
+      </c>
+      <c r="D17">
+        <v>0.81481000000000003</v>
+      </c>
+      <c r="E17">
+        <v>0.81481000000000003</v>
+      </c>
+      <c r="F17">
+        <v>0.85185</v>
+      </c>
+      <c r="G17">
+        <v>0.74026000000000003</v>
+      </c>
+      <c r="H17">
+        <v>0.72726999999999997</v>
+      </c>
+      <c r="I17">
+        <v>0.71428999999999998</v>
+      </c>
+      <c r="J17">
+        <v>0.75294000000000005</v>
+      </c>
+      <c r="K17">
+        <v>0.76471</v>
+      </c>
+      <c r="L17">
+        <v>0.78824000000000005</v>
+      </c>
+      <c r="M17">
+        <v>0.91769999999999996</v>
+      </c>
+      <c r="N17">
+        <v>0.91925000000000001</v>
+      </c>
+      <c r="O17">
+        <v>0.91303999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>0.61904999999999999</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.61904999999999999</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.61904999999999999</v>
+      </c>
+      <c r="D18">
+        <v>0.70369999999999999</v>
+      </c>
+      <c r="E18">
         <v>0.66666999999999998</v>
       </c>
-      <c r="G16">
-        <v>0.68830999999999998</v>
-      </c>
-      <c r="H16">
-        <v>0.70130000000000003</v>
-      </c>
-      <c r="I16">
-        <v>0.70130000000000003</v>
-      </c>
-      <c r="J16">
-        <v>0.77646999999999999</v>
-      </c>
-      <c r="K16">
-        <v>0.78824000000000005</v>
-      </c>
-      <c r="L16">
-        <v>0.81176000000000004</v>
-      </c>
-      <c r="M16">
-        <v>0.91303999999999996</v>
-      </c>
-      <c r="N16">
-        <v>0.90993999999999997</v>
-      </c>
-      <c r="O16">
-        <v>0.92701999999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A17" s="1">
-        <v>0.68181999999999998</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0.72726999999999997</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.72726999999999997</v>
-      </c>
-      <c r="D17">
-        <v>0.88888999999999996</v>
-      </c>
-      <c r="E17">
-        <v>0.88888999999999996</v>
-      </c>
-      <c r="F17">
-        <v>0.92593000000000003</v>
-      </c>
-      <c r="G17">
-        <v>0.75324999999999998</v>
-      </c>
-      <c r="H17">
-        <v>0.81818000000000002</v>
-      </c>
-      <c r="I17">
+      <c r="F18">
+        <v>0.70369999999999999</v>
+      </c>
+      <c r="G18">
         <v>0.77922000000000002</v>
       </c>
-      <c r="J17">
-        <v>0.88234999999999997</v>
-      </c>
-      <c r="K17">
-        <v>0.88234999999999997</v>
-      </c>
-      <c r="L17">
-        <v>0.75294000000000005</v>
-      </c>
-      <c r="M17">
-        <v>0.92391000000000001</v>
-      </c>
-      <c r="N17">
-        <v>0.92547000000000001</v>
-      </c>
-      <c r="O17">
-        <v>0.90839000000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A18" s="1">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="B18" s="1">
-        <v>0.80952000000000002</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="D18">
-        <v>0.88888999999999996</v>
-      </c>
-      <c r="E18">
-        <v>0.88888999999999996</v>
-      </c>
-      <c r="F18">
-        <v>0.81481000000000003</v>
-      </c>
-      <c r="G18">
-        <v>0.72726999999999997</v>
-      </c>
       <c r="H18">
-        <v>0.75324999999999998</v>
+        <v>0.80518999999999996</v>
       </c>
       <c r="I18">
-        <v>0.70130000000000003</v>
+        <v>0.80518999999999996</v>
       </c>
       <c r="J18">
         <v>0.71765000000000001</v>
       </c>
       <c r="K18">
+        <v>0.76471</v>
+      </c>
+      <c r="L18">
+        <v>0.70587999999999995</v>
+      </c>
+      <c r="M18">
+        <v>0.91459999999999997</v>
+      </c>
+      <c r="N18">
+        <v>0.90993999999999997</v>
+      </c>
+      <c r="O18">
+        <v>0.90683000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>0.71428999999999998</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.61904999999999999</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.71428999999999998</v>
+      </c>
+      <c r="D19">
+        <v>0.70369999999999999</v>
+      </c>
+      <c r="E19">
+        <v>0.62963000000000002</v>
+      </c>
+      <c r="F19">
+        <v>0.66666999999999998</v>
+      </c>
+      <c r="G19">
+        <v>0.75324999999999998</v>
+      </c>
+      <c r="H19">
+        <v>0.77922000000000002</v>
+      </c>
+      <c r="I19">
+        <v>0.76622999999999997</v>
+      </c>
+      <c r="J19">
         <v>0.69411999999999996</v>
       </c>
-      <c r="L18">
-        <v>0.67059000000000002</v>
-      </c>
-      <c r="M18">
-        <v>0.90061999999999998</v>
-      </c>
-      <c r="N18">
-        <v>0.89595999999999998</v>
-      </c>
-      <c r="O18">
-        <v>0.91925000000000001</v>
+      <c r="K19">
+        <v>0.69411999999999996</v>
+      </c>
+      <c r="L19">
+        <v>0.75294000000000005</v>
+      </c>
+      <c r="M19">
+        <v>0.90824000000000005</v>
+      </c>
+      <c r="N19">
+        <v>0.90669</v>
+      </c>
+      <c r="O19">
+        <v>0.89890999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A19" s="1">
-        <v>0.80952000000000002</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0.90476000000000001</v>
-      </c>
-      <c r="D19">
-        <v>0.77778000000000003</v>
-      </c>
-      <c r="E19">
-        <v>0.74073999999999995</v>
-      </c>
-      <c r="F19">
-        <v>0.81481000000000003</v>
-      </c>
-      <c r="G19">
-        <v>0.79220999999999997</v>
-      </c>
-      <c r="H19">
-        <v>0.75324999999999998</v>
-      </c>
-      <c r="I19">
-        <v>0.74026000000000003</v>
-      </c>
-      <c r="J19">
-        <v>0.72941</v>
-      </c>
-      <c r="K19">
-        <v>0.72941</v>
-      </c>
-      <c r="L19">
-        <v>0.72941</v>
-      </c>
-      <c r="M19">
-        <v>0.92068000000000005</v>
-      </c>
-      <c r="N19">
-        <v>0.92223999999999995</v>
-      </c>
-      <c r="O19">
-        <v>0.90046999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>0.85714000000000001</v>
       </c>
       <c r="B20" s="1">
+        <v>0.95238</v>
+      </c>
+      <c r="C20" s="1">
         <v>0.80952000000000002</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0.76190000000000002</v>
       </c>
       <c r="D20">
         <v>0.81481000000000003</v>
       </c>
       <c r="E20">
+        <v>0.85185</v>
+      </c>
+      <c r="F20">
         <v>0.81481000000000003</v>
       </c>
-      <c r="F20">
-        <v>0.88888999999999996</v>
-      </c>
       <c r="G20">
-        <v>0.70130000000000003</v>
+        <v>0.79220999999999997</v>
       </c>
       <c r="H20">
-        <v>0.70130000000000003</v>
+        <v>0.77922000000000002</v>
       </c>
       <c r="I20">
-        <v>0.74026000000000003</v>
+        <v>0.79220999999999997</v>
       </c>
       <c r="J20">
-        <v>0.72619</v>
+        <v>0.78571000000000002</v>
       </c>
       <c r="K20">
-        <v>0.72619</v>
+        <v>0.78571000000000002</v>
       </c>
       <c r="L20">
-        <v>0.73809999999999998</v>
+        <v>0.80952000000000002</v>
       </c>
       <c r="M20">
-        <v>0.90046999999999999</v>
+        <v>0.90980000000000005</v>
       </c>
       <c r="N20">
-        <v>0.90202000000000004</v>
+        <v>0.89736000000000005</v>
       </c>
       <c r="O20">
-        <v>0.91134999999999999</v>
+        <v>0.90358000000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>0.76190000000000002</v>
+        <v>0.80952000000000002</v>
       </c>
       <c r="B21" s="1">
-        <v>0.76190000000000002</v>
+        <v>0.90476000000000001</v>
       </c>
       <c r="C21" s="1">
-        <v>0.71428999999999998</v>
+        <v>0.85714000000000001</v>
       </c>
       <c r="D21">
-        <v>0.70369999999999999</v>
+        <v>0.85185</v>
       </c>
       <c r="E21">
-        <v>0.70369999999999999</v>
+        <v>0.85185</v>
       </c>
       <c r="F21">
         <v>0.85185</v>
       </c>
       <c r="G21">
-        <v>0.72726999999999997</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="H21">
+        <v>0.74026000000000003</v>
+      </c>
+      <c r="I21">
         <v>0.75324999999999998</v>
       </c>
-      <c r="I21">
-        <v>0.72726999999999997</v>
-      </c>
       <c r="J21">
-        <v>0.78571000000000002</v>
+        <v>0.72619</v>
       </c>
       <c r="K21">
+        <v>0.72619</v>
+      </c>
+      <c r="L21">
+        <v>0.73809999999999998</v>
+      </c>
+      <c r="M21">
+        <v>0.91757</v>
+      </c>
+      <c r="N21">
+        <v>0.91913</v>
+      </c>
+      <c r="O21">
+        <v>0.92535000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>0.80952000000000002</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.80952000000000002</v>
+      </c>
+      <c r="C22" s="1">
         <v>0.76190000000000002</v>
-      </c>
-      <c r="L21">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="M21">
-        <v>0.91291</v>
-      </c>
-      <c r="N21">
-        <v>0.90980000000000005</v>
-      </c>
-      <c r="O21">
-        <v>0.90358000000000005</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A22" s="1">
-        <v>0.85714000000000001</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.85714000000000001</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0.71428999999999998</v>
       </c>
       <c r="D22">
         <v>0.96296000000000004</v>
@@ -4530,96 +4710,96 @@
         <v>0.96296000000000004</v>
       </c>
       <c r="F22">
-        <v>0.85185</v>
+        <v>0.92593000000000003</v>
       </c>
       <c r="G22">
-        <v>0.80262999999999995</v>
+        <v>0.69737000000000005</v>
       </c>
       <c r="H22">
-        <v>0.78947000000000001</v>
+        <v>0.72367999999999999</v>
       </c>
       <c r="I22">
-        <v>0.80262999999999995</v>
+        <v>0.69737000000000005</v>
       </c>
       <c r="J22">
+        <v>0.77381</v>
+      </c>
+      <c r="K22">
         <v>0.76190000000000002</v>
       </c>
-      <c r="K22">
-        <v>0.79762</v>
-      </c>
       <c r="L22">
-        <v>0.66666999999999998</v>
+        <v>0.76190000000000002</v>
       </c>
       <c r="M22">
-        <v>0.90824000000000005</v>
+        <v>0.91757</v>
       </c>
       <c r="N22">
-        <v>0.90669</v>
+        <v>0.92223999999999995</v>
       </c>
       <c r="O22">
-        <v>0.89890999999999999</v>
+        <v>0.91757</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <f>AVERAGE(A3:A22) * 100</f>
-        <v>75.508550000000014</v>
+        <v>79.458799999999982</v>
       </c>
       <c r="B23">
         <f t="shared" ref="B23:O23" si="0">AVERAGE(B3:B22) * 100</f>
-        <v>74.794300000000007</v>
+        <v>77.370099999999994</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>75.952250000000006</v>
+        <v>77.57565000000001</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>84.444400000000002</v>
+        <v>82.22199999999998</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>82.777699999999996</v>
+        <v>81.666550000000001</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>82.222200000000001</v>
+        <v>81.851800000000011</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>74.943550000000002</v>
+        <v>76.100500000000011</v>
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
-        <v>74.618149999999986</v>
+        <v>75.516099999999994</v>
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>74.161799999999999</v>
+        <v>75.58359999999999</v>
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>75.591000000000008</v>
+        <v>75.070150000000012</v>
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>75.709400000000016</v>
+        <v>75.240950000000012</v>
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
-        <v>73.65055000000001</v>
+        <v>75.06795000000001</v>
       </c>
       <c r="M23">
         <f t="shared" si="0"/>
-        <v>91.748199999999997</v>
+        <v>91.623800000000017</v>
       </c>
       <c r="N23">
         <f t="shared" si="0"/>
-        <v>91.538500000000028</v>
+        <v>91.367499999999993</v>
       </c>
       <c r="O23">
         <f t="shared" si="0"/>
-        <v>90.730400000000017</v>
+        <v>91.382900000000035</v>
       </c>
     </row>
   </sheetData>
@@ -4635,12 +4815,12 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4667,7 +4847,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -4678,244 +4858,244 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>0.71428999999999998</v>
+        <v>0.90476000000000001</v>
       </c>
       <c r="B3" s="1">
-        <v>0.76190000000000002</v>
+        <v>0.95238</v>
       </c>
       <c r="C3" s="1">
-        <v>0.80952000000000002</v>
+        <v>0.90476000000000001</v>
       </c>
       <c r="D3">
-        <v>0.92593000000000003</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="E3" s="1">
         <v>0.85185</v>
       </c>
       <c r="F3">
-        <v>0.77778000000000003</v>
+        <v>0.85185</v>
       </c>
       <c r="G3">
         <v>0.77632000000000001</v>
       </c>
       <c r="H3">
-        <v>0.73684000000000005</v>
+        <v>0.76315999999999995</v>
       </c>
       <c r="I3">
         <v>0.75</v>
       </c>
       <c r="J3">
+        <v>0.70238</v>
+      </c>
+      <c r="K3">
         <v>0.72619</v>
       </c>
-      <c r="K3">
-        <v>0.77381</v>
-      </c>
       <c r="L3">
-        <v>0.85714000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="M3">
-        <v>0.91757</v>
+        <v>0.92535000000000001</v>
       </c>
       <c r="N3">
-        <v>0.90358000000000005</v>
+        <v>0.91291</v>
       </c>
       <c r="O3">
-        <v>0.92068000000000005</v>
+        <v>0.91913</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>0.5</v>
+        <v>0.77273000000000003</v>
       </c>
       <c r="B4" s="1">
-        <v>0.54544999999999999</v>
+        <v>0.77273000000000003</v>
       </c>
       <c r="C4" s="1">
-        <v>0.81818000000000002</v>
+        <v>0.77273000000000003</v>
       </c>
       <c r="D4">
         <v>0.88888999999999996</v>
       </c>
       <c r="E4" s="1">
-        <v>0.85185</v>
+        <v>0.92593000000000003</v>
       </c>
       <c r="F4">
-        <v>0.77778000000000003</v>
+        <v>0.88888999999999996</v>
       </c>
       <c r="G4">
-        <v>0.72726999999999997</v>
+        <v>0.64934999999999998</v>
       </c>
       <c r="H4">
-        <v>0.76622999999999997</v>
+        <v>0.68830999999999998</v>
       </c>
       <c r="I4">
-        <v>0.72726999999999997</v>
+        <v>0.64934999999999998</v>
       </c>
       <c r="J4">
-        <v>0.74117999999999995</v>
+        <v>0.69411999999999996</v>
       </c>
       <c r="K4">
-        <v>0.75294000000000005</v>
+        <v>0.70587999999999995</v>
       </c>
       <c r="L4">
-        <v>0.74117999999999995</v>
+        <v>0.71765000000000001</v>
       </c>
       <c r="M4">
-        <v>0.92701999999999996</v>
+        <v>0.91615000000000002</v>
       </c>
       <c r="N4">
         <v>0.91303999999999996</v>
       </c>
       <c r="O4">
-        <v>0.91149000000000002</v>
+        <v>0.91303999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
+        <v>0.81818000000000002</v>
+      </c>
+      <c r="B5" s="1">
         <v>0.77273000000000003</v>
       </c>
-      <c r="B5" s="1">
-        <v>0.72726999999999997</v>
-      </c>
       <c r="C5" s="1">
-        <v>0.72726999999999997</v>
+        <v>0.86363999999999996</v>
       </c>
       <c r="D5">
-        <v>0.77778000000000003</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="E5" s="1">
         <v>0.81481000000000003</v>
       </c>
       <c r="F5">
-        <v>0.74073999999999995</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="G5">
-        <v>0.76622999999999997</v>
+        <v>0.77922000000000002</v>
       </c>
       <c r="H5">
-        <v>0.75324999999999998</v>
+        <v>0.77922000000000002</v>
       </c>
       <c r="I5">
-        <v>0.77922000000000002</v>
+        <v>0.74026000000000003</v>
       </c>
       <c r="J5">
-        <v>0.78824000000000005</v>
+        <v>0.70587999999999995</v>
       </c>
       <c r="K5">
-        <v>0.77646999999999999</v>
+        <v>0.71765000000000001</v>
       </c>
       <c r="L5">
-        <v>0.75294000000000005</v>
+        <v>0.69411999999999996</v>
       </c>
       <c r="M5">
-        <v>0.91149000000000002</v>
+        <v>0.91459999999999997</v>
       </c>
       <c r="N5">
-        <v>0.90683000000000002</v>
+        <v>0.91303999999999996</v>
       </c>
       <c r="O5">
-        <v>0.91615000000000002</v>
+        <v>0.91459999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>0.77273000000000003</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="B6" s="1">
-        <v>0.68181999999999998</v>
+        <v>0.72726999999999997</v>
       </c>
       <c r="C6" s="1">
-        <v>0.77273000000000003</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="D6">
-        <v>0.85185</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="E6" s="1">
-        <v>0.85185</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="F6">
-        <v>0.85185</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="G6">
         <v>0.80518999999999996</v>
       </c>
       <c r="H6">
-        <v>0.84416000000000002</v>
+        <v>0.80518999999999996</v>
       </c>
       <c r="I6">
-        <v>0.70130000000000003</v>
+        <v>0.79220999999999997</v>
       </c>
       <c r="J6">
-        <v>0.68235000000000001</v>
+        <v>0.71765000000000001</v>
       </c>
       <c r="K6">
-        <v>0.68235000000000001</v>
+        <v>0.74117999999999995</v>
       </c>
       <c r="L6">
-        <v>0.74117999999999995</v>
+        <v>0.71765000000000001</v>
       </c>
       <c r="M6">
-        <v>0.90839000000000003</v>
+        <v>0.89751999999999998</v>
       </c>
       <c r="N6">
-        <v>0.91303999999999996</v>
+        <v>0.90061999999999998</v>
       </c>
       <c r="O6">
-        <v>0.92857000000000001</v>
+        <v>0.90217000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>0.72726999999999997</v>
+        <v>0.59091000000000005</v>
       </c>
       <c r="B7" s="1">
-        <v>0.77273000000000003</v>
+        <v>0.63636000000000004</v>
       </c>
       <c r="C7" s="1">
-        <v>0.68181999999999998</v>
+        <v>0.59091000000000005</v>
       </c>
       <c r="D7">
-        <v>0.85185</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="E7" s="1">
-        <v>0.74073999999999995</v>
+        <v>0.77778000000000003</v>
       </c>
       <c r="F7">
-        <v>0.81481000000000003</v>
+        <v>0.77778000000000003</v>
       </c>
       <c r="G7">
-        <v>0.70130000000000003</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="H7">
-        <v>0.70130000000000003</v>
+        <v>0.74026000000000003</v>
       </c>
       <c r="I7">
-        <v>0.76622999999999997</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="J7">
-        <v>0.64705999999999997</v>
+        <v>0.71765000000000001</v>
       </c>
       <c r="K7">
+        <v>0.69411999999999996</v>
+      </c>
+      <c r="L7">
         <v>0.71765000000000001</v>
       </c>
-      <c r="L7">
-        <v>0.70587999999999995</v>
-      </c>
       <c r="M7">
-        <v>0.89441000000000004</v>
+        <v>0.90373000000000003</v>
       </c>
       <c r="N7">
-        <v>0.89441000000000004</v>
+        <v>0.89907000000000004</v>
       </c>
       <c r="O7">
         <v>0.91303999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>0.66666999999999998</v>
+        <v>0.80952000000000002</v>
       </c>
       <c r="B8" s="1">
         <v>0.80952000000000002</v>
@@ -4924,10 +5104,10 @@
         <v>0.76190000000000002</v>
       </c>
       <c r="D8">
-        <v>0.88888999999999996</v>
+        <v>0.77778000000000003</v>
       </c>
       <c r="E8" s="1">
-        <v>0.88888999999999996</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="F8">
         <v>0.81481000000000003</v>
@@ -4936,277 +5116,277 @@
         <v>0.79220999999999997</v>
       </c>
       <c r="H8">
-        <v>0.79220999999999997</v>
+        <v>0.77922000000000002</v>
       </c>
       <c r="I8">
-        <v>0.74026000000000003</v>
+        <v>0.77922000000000002</v>
       </c>
       <c r="J8">
-        <v>0.78824000000000005</v>
+        <v>0.75294000000000005</v>
       </c>
       <c r="K8">
         <v>0.76471</v>
       </c>
       <c r="L8">
+        <v>0.72941</v>
+      </c>
+      <c r="M8">
+        <v>0.91925000000000001</v>
+      </c>
+      <c r="N8">
+        <v>0.91149000000000002</v>
+      </c>
+      <c r="O8">
+        <v>0.91925000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>0.85714000000000001</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.85714000000000001</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.85714000000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.81481000000000003</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.77778000000000003</v>
+      </c>
+      <c r="F9">
+        <v>0.85185</v>
+      </c>
+      <c r="G9">
+        <v>0.68830999999999998</v>
+      </c>
+      <c r="H9">
+        <v>0.68830999999999998</v>
+      </c>
+      <c r="I9">
+        <v>0.74026000000000003</v>
+      </c>
+      <c r="J9">
         <v>0.68235000000000001</v>
-      </c>
-      <c r="M8">
-        <v>0.92081000000000002</v>
-      </c>
-      <c r="N8">
-        <v>0.91925000000000001</v>
-      </c>
-      <c r="O8">
-        <v>0.93478000000000006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A9" s="1">
-        <v>0.71428999999999998</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.80952000000000002</v>
-      </c>
-      <c r="D9">
-        <v>0.92593000000000003</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.85185</v>
-      </c>
-      <c r="F9">
-        <v>0.96296000000000004</v>
-      </c>
-      <c r="G9">
-        <v>0.75324999999999998</v>
-      </c>
-      <c r="H9">
-        <v>0.76622999999999997</v>
-      </c>
-      <c r="I9">
-        <v>0.76622999999999997</v>
-      </c>
-      <c r="J9">
-        <v>0.72941</v>
       </c>
       <c r="K9">
         <v>0.71765000000000001</v>
       </c>
       <c r="L9">
-        <v>0.77646999999999999</v>
+        <v>0.75294000000000005</v>
       </c>
       <c r="M9">
-        <v>0.91757</v>
+        <v>0.90824000000000005</v>
       </c>
       <c r="N9">
-        <v>0.90980000000000005</v>
+        <v>0.91134999999999999</v>
       </c>
       <c r="O9">
-        <v>0.90202000000000004</v>
+        <v>0.90824000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
+        <v>0.80952000000000002</v>
+      </c>
+      <c r="B10" s="1">
         <v>0.76190000000000002</v>
       </c>
-      <c r="B10" s="1">
-        <v>0.66666999999999998</v>
-      </c>
       <c r="C10" s="1">
-        <v>0.66666999999999998</v>
+        <v>0.76190000000000002</v>
       </c>
       <c r="D10">
+        <v>0.85185</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.85185</v>
+      </c>
+      <c r="F10">
         <v>0.81481000000000003</v>
       </c>
-      <c r="E10" s="1">
+      <c r="G10">
+        <v>0.81818000000000002</v>
+      </c>
+      <c r="H10">
+        <v>0.79220999999999997</v>
+      </c>
+      <c r="I10">
+        <v>0.80518999999999996</v>
+      </c>
+      <c r="J10">
+        <v>0.75</v>
+      </c>
+      <c r="K10">
+        <v>0.75</v>
+      </c>
+      <c r="L10">
+        <v>0.77381</v>
+      </c>
+      <c r="M10">
+        <v>0.93001999999999996</v>
+      </c>
+      <c r="N10">
+        <v>0.92379</v>
+      </c>
+      <c r="O10">
+        <v>0.92691000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>0.85714000000000001</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.90476000000000001</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.80952000000000002</v>
+      </c>
+      <c r="D11">
         <v>0.74073999999999995</v>
-      </c>
-      <c r="F10">
-        <v>0.85185</v>
-      </c>
-      <c r="G10">
-        <v>0.77922000000000002</v>
-      </c>
-      <c r="H10">
-        <v>0.77922000000000002</v>
-      </c>
-      <c r="I10">
-        <v>0.74026000000000003</v>
-      </c>
-      <c r="J10">
-        <v>0.73809999999999998</v>
-      </c>
-      <c r="K10">
-        <v>0.71428999999999998</v>
-      </c>
-      <c r="L10">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="M10">
-        <v>0.92223999999999995</v>
-      </c>
-      <c r="N10">
-        <v>0.91757</v>
-      </c>
-      <c r="O10">
-        <v>0.90358000000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A11" s="1">
-        <v>0.61904999999999999</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.61904999999999999</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="D11">
-        <v>0.77778000000000003</v>
       </c>
       <c r="E11" s="1">
         <v>0.77778000000000003</v>
       </c>
       <c r="F11">
-        <v>0.81481000000000003</v>
+        <v>0.85185</v>
       </c>
       <c r="G11">
-        <v>0.72726999999999997</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="H11">
-        <v>0.72726999999999997</v>
+        <v>0.76622999999999997</v>
       </c>
       <c r="I11">
-        <v>0.77922000000000002</v>
+        <v>0.74026000000000003</v>
       </c>
       <c r="J11">
-        <v>0.83333000000000002</v>
+        <v>0.82142999999999999</v>
       </c>
       <c r="K11">
-        <v>0.78571000000000002</v>
+        <v>0.73809999999999998</v>
       </c>
       <c r="L11">
+        <v>0.79762</v>
+      </c>
+      <c r="M11">
+        <v>0.90669</v>
+      </c>
+      <c r="N11">
+        <v>0.90980000000000005</v>
+      </c>
+      <c r="O11">
+        <v>0.91291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>0.57142999999999999</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.52381</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.57142999999999999</v>
+      </c>
+      <c r="D12">
+        <v>0.92593000000000003</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.96296000000000004</v>
+      </c>
+      <c r="F12">
+        <v>0.88888999999999996</v>
+      </c>
+      <c r="G12">
+        <v>0.77632000000000001</v>
+      </c>
+      <c r="H12">
+        <v>0.80262999999999995</v>
+      </c>
+      <c r="I12">
+        <v>0.80262999999999995</v>
+      </c>
+      <c r="J12">
+        <v>0.79762</v>
+      </c>
+      <c r="K12">
         <v>0.76190000000000002</v>
       </c>
-      <c r="M11">
-        <v>0.90980000000000005</v>
-      </c>
-      <c r="N11">
-        <v>0.90512999999999999</v>
-      </c>
-      <c r="O11">
-        <v>0.90512999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A12" s="1">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0.85714000000000001</v>
-      </c>
-      <c r="D12">
-        <v>0.74073999999999995</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.77778000000000003</v>
-      </c>
-      <c r="F12">
-        <v>0.85185</v>
-      </c>
-      <c r="G12">
-        <v>0.75</v>
-      </c>
-      <c r="H12">
-        <v>0.76315999999999995</v>
-      </c>
-      <c r="I12">
-        <v>0.84211000000000003</v>
-      </c>
-      <c r="J12">
-        <v>0.76190000000000002</v>
-      </c>
-      <c r="K12">
-        <v>0.71428999999999998</v>
-      </c>
       <c r="L12">
-        <v>0.71428999999999998</v>
+        <v>0.80952000000000002</v>
       </c>
       <c r="M12">
-        <v>0.91446000000000005</v>
+        <v>0.89580000000000004</v>
       </c>
       <c r="N12">
         <v>0.89736000000000005</v>
       </c>
       <c r="O12">
-        <v>0.92379</v>
+        <v>0.89114000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>0.85714000000000001</v>
+        <v>0.76190000000000002</v>
       </c>
       <c r="B13" s="1">
-        <v>0.90476000000000001</v>
+        <v>0.76190000000000002</v>
       </c>
       <c r="C13" s="1">
-        <v>0.85714000000000001</v>
+        <v>0.76190000000000002</v>
       </c>
       <c r="D13">
-        <v>0.74073999999999995</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="E13" s="1">
         <v>0.81481000000000003</v>
       </c>
       <c r="F13">
-        <v>0.74073999999999995</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="G13">
-        <v>0.77632000000000001</v>
+        <v>0.72367999999999999</v>
       </c>
       <c r="H13">
-        <v>0.80262999999999995</v>
+        <v>0.73684000000000005</v>
       </c>
       <c r="I13">
         <v>0.75</v>
       </c>
       <c r="J13">
-        <v>0.73809999999999998</v>
+        <v>0.69047999999999998</v>
       </c>
       <c r="K13">
-        <v>0.77381</v>
+        <v>0.67857000000000001</v>
       </c>
       <c r="L13">
-        <v>0.73809999999999998</v>
+        <v>0.72619</v>
       </c>
       <c r="M13">
-        <v>0.93313000000000001</v>
+        <v>0.91291</v>
       </c>
       <c r="N13">
-        <v>0.92223999999999995</v>
+        <v>0.90669</v>
       </c>
       <c r="O13">
-        <v>0.90824000000000005</v>
+        <v>0.90669</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>0.77273000000000003</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="B14" s="1">
-        <v>0.77273000000000003</v>
+        <v>0.90908999999999995</v>
       </c>
       <c r="C14" s="1">
-        <v>0.77273000000000003</v>
+        <v>0.90908999999999995</v>
       </c>
       <c r="D14">
-        <v>0.81481000000000003</v>
+        <v>0.77778000000000003</v>
       </c>
       <c r="E14" s="1">
         <v>0.81481000000000003</v>
@@ -5215,269 +5395,269 @@
         <v>0.81481000000000003</v>
       </c>
       <c r="G14">
-        <v>0.72726999999999997</v>
+        <v>0.79220999999999997</v>
       </c>
       <c r="H14">
         <v>0.71428999999999998</v>
       </c>
       <c r="I14">
-        <v>0.63636000000000004</v>
+        <v>0.71428999999999998</v>
       </c>
       <c r="J14">
-        <v>0.72941</v>
+        <v>0.74117999999999995</v>
       </c>
       <c r="K14">
-        <v>0.71765000000000001</v>
+        <v>0.70587999999999995</v>
       </c>
       <c r="L14">
-        <v>0.74117999999999995</v>
+        <v>0.68235000000000001</v>
       </c>
       <c r="M14">
-        <v>0.92857000000000001</v>
+        <v>0.91925000000000001</v>
       </c>
       <c r="N14">
-        <v>0.91925000000000001</v>
+        <v>0.90993999999999997</v>
       </c>
       <c r="O14">
-        <v>0.90373000000000003</v>
+        <v>0.91459999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>0.72726999999999997</v>
+        <v>0.77273000000000003</v>
       </c>
       <c r="B15" s="1">
-        <v>0.72726999999999997</v>
+        <v>0.77273000000000003</v>
       </c>
       <c r="C15" s="1">
-        <v>0.72726999999999997</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="D15">
         <v>0.81481000000000003</v>
       </c>
       <c r="E15" s="1">
-        <v>0.85185</v>
+        <v>0.77778000000000003</v>
       </c>
       <c r="F15">
         <v>0.81481000000000003</v>
       </c>
       <c r="G15">
-        <v>0.68830999999999998</v>
+        <v>0.76622999999999997</v>
       </c>
       <c r="H15">
-        <v>0.71428999999999998</v>
+        <v>0.79220999999999997</v>
       </c>
       <c r="I15">
-        <v>0.72726999999999997</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="J15">
-        <v>0.74117999999999995</v>
+        <v>0.77646999999999999</v>
       </c>
       <c r="K15">
-        <v>0.75294000000000005</v>
+        <v>0.77646999999999999</v>
       </c>
       <c r="L15">
-        <v>0.75294000000000005</v>
+        <v>0.76471</v>
       </c>
       <c r="M15">
+        <v>0.92701999999999996</v>
+      </c>
+      <c r="N15">
+        <v>0.91925000000000001</v>
+      </c>
+      <c r="O15">
         <v>0.92081000000000002</v>
       </c>
-      <c r="N15">
-        <v>0.92081000000000002</v>
-      </c>
-      <c r="O15">
-        <v>0.90061999999999998</v>
-      </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>0.77273000000000003</v>
+        <v>0.68181999999999998</v>
       </c>
       <c r="B16" s="1">
-        <v>0.77273000000000003</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="C16" s="1">
-        <v>0.72726999999999997</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="D16">
-        <v>0.92593000000000003</v>
+        <v>0.74073999999999995</v>
       </c>
       <c r="E16" s="1">
-        <v>0.85185</v>
+        <v>0.70369999999999999</v>
       </c>
       <c r="F16">
-        <v>0.74073999999999995</v>
+        <v>0.66666999999999998</v>
       </c>
       <c r="G16">
-        <v>0.77922000000000002</v>
+        <v>0.76622999999999997</v>
       </c>
       <c r="H16">
-        <v>0.75324999999999998</v>
+        <v>0.76622999999999997</v>
       </c>
       <c r="I16">
         <v>0.75324999999999998</v>
       </c>
       <c r="J16">
-        <v>0.74117999999999995</v>
+        <v>0.77646999999999999</v>
       </c>
       <c r="K16">
-        <v>0.74117999999999995</v>
+        <v>0.77646999999999999</v>
       </c>
       <c r="L16">
-        <v>0.76471</v>
+        <v>0.77646999999999999</v>
       </c>
       <c r="M16">
-        <v>0.90993999999999997</v>
+        <v>0.92235999999999996</v>
       </c>
       <c r="N16">
-        <v>0.91303999999999996</v>
+        <v>0.91925000000000001</v>
       </c>
       <c r="O16">
-        <v>0.92235999999999996</v>
+        <v>0.91615000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>0.72726999999999997</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="B17" s="1">
-        <v>0.77273000000000003</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="C17" s="1">
-        <v>0.72726999999999997</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="D17">
-        <v>0.81481000000000003</v>
+        <v>0.77778000000000003</v>
       </c>
       <c r="E17" s="1">
-        <v>0.81481000000000003</v>
+        <v>0.77778000000000003</v>
       </c>
       <c r="F17">
-        <v>0.92593000000000003</v>
+        <v>0.77778000000000003</v>
       </c>
       <c r="G17">
-        <v>0.72726999999999997</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="H17">
-        <v>0.72726999999999997</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="I17">
-        <v>0.80518999999999996</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="J17">
-        <v>0.82352999999999998</v>
+        <v>0.72941</v>
       </c>
       <c r="K17">
         <v>0.77646999999999999</v>
       </c>
       <c r="L17">
-        <v>0.75294000000000005</v>
+        <v>0.77646999999999999</v>
       </c>
       <c r="M17">
-        <v>0.92857000000000001</v>
+        <v>0.91303999999999996</v>
       </c>
       <c r="N17">
-        <v>0.92701999999999996</v>
+        <v>0.90839000000000003</v>
       </c>
       <c r="O17">
-        <v>0.92081000000000002</v>
+        <v>0.90839000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>0.76190000000000002</v>
+        <v>0.66666999999999998</v>
       </c>
       <c r="B18" s="1">
         <v>0.76190000000000002</v>
       </c>
       <c r="C18" s="1">
-        <v>0.71428999999999998</v>
+        <v>0.76190000000000002</v>
       </c>
       <c r="D18">
-        <v>0.88888999999999996</v>
+        <v>0.66666999999999998</v>
       </c>
       <c r="E18" s="1">
-        <v>0.85185</v>
+        <v>0.66666999999999998</v>
       </c>
       <c r="F18">
-        <v>0.85185</v>
+        <v>0.66666999999999998</v>
       </c>
       <c r="G18">
-        <v>0.76622999999999997</v>
+        <v>0.79220999999999997</v>
       </c>
       <c r="H18">
-        <v>0.68830999999999998</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="I18">
-        <v>0.75324999999999998</v>
+        <v>0.77922000000000002</v>
       </c>
       <c r="J18">
-        <v>0.71765000000000001</v>
+        <v>0.72941</v>
       </c>
       <c r="K18">
-        <v>0.75294000000000005</v>
+        <v>0.68235000000000001</v>
       </c>
       <c r="L18">
         <v>0.67059000000000002</v>
       </c>
       <c r="M18">
-        <v>0.89907000000000004</v>
+        <v>0.91459999999999997</v>
       </c>
       <c r="N18">
-        <v>0.89907000000000004</v>
+        <v>0.90993999999999997</v>
       </c>
       <c r="O18">
-        <v>0.92391000000000001</v>
+        <v>0.90839000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>0.76190000000000002</v>
+        <v>0.66666999999999998</v>
       </c>
       <c r="B19" s="1">
-        <v>0.76190000000000002</v>
+        <v>0.61904999999999999</v>
       </c>
       <c r="C19" s="1">
-        <v>0.85714000000000001</v>
+        <v>0.66666999999999998</v>
       </c>
       <c r="D19">
+        <v>0.74073999999999995</v>
+      </c>
+      <c r="E19" s="1">
         <v>0.81481000000000003</v>
       </c>
-      <c r="E19" s="1">
-        <v>0.70369999999999999</v>
-      </c>
       <c r="F19">
-        <v>0.85185</v>
+        <v>0.81481000000000003</v>
       </c>
       <c r="G19">
-        <v>0.76622999999999997</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="H19">
-        <v>0.74026000000000003</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="I19">
-        <v>0.74026000000000003</v>
+        <v>0.72726999999999997</v>
       </c>
       <c r="J19">
-        <v>0.77646999999999999</v>
+        <v>0.76471</v>
       </c>
       <c r="K19">
-        <v>0.75294000000000005</v>
+        <v>0.72941</v>
       </c>
       <c r="L19">
-        <v>0.75294000000000005</v>
+        <v>0.76471</v>
       </c>
       <c r="M19">
-        <v>0.91291</v>
+        <v>0.90202000000000004</v>
       </c>
       <c r="N19">
-        <v>0.90358000000000005</v>
+        <v>0.90512999999999999</v>
       </c>
       <c r="O19">
-        <v>0.91134999999999999</v>
+        <v>0.90202000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>0.90476000000000001</v>
       </c>
@@ -5485,57 +5665,57 @@
         <v>0.85714000000000001</v>
       </c>
       <c r="C20" s="1">
-        <v>0.80952000000000002</v>
+        <v>0.90476000000000001</v>
       </c>
       <c r="D20">
-        <v>0.81481000000000003</v>
+        <v>0.77778000000000003</v>
       </c>
       <c r="E20" s="1">
         <v>0.81481000000000003</v>
       </c>
       <c r="F20">
-        <v>0.88888999999999996</v>
+        <v>0.77778000000000003</v>
       </c>
       <c r="G20">
-        <v>0.80518999999999996</v>
+        <v>0.81818000000000002</v>
       </c>
       <c r="H20">
         <v>0.76622999999999997</v>
       </c>
       <c r="I20">
-        <v>0.70130000000000003</v>
+        <v>0.75324999999999998</v>
       </c>
       <c r="J20">
-        <v>0.72619</v>
+        <v>0.77381</v>
       </c>
       <c r="K20">
-        <v>0.75</v>
+        <v>0.79762</v>
       </c>
       <c r="L20">
-        <v>0.75</v>
+        <v>0.82142999999999999</v>
       </c>
       <c r="M20">
-        <v>0.89424999999999999</v>
+        <v>0.90358000000000005</v>
       </c>
       <c r="N20">
-        <v>0.89114000000000004</v>
+        <v>0.91291</v>
       </c>
       <c r="O20">
-        <v>0.92379</v>
+        <v>0.90202000000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>0.76190000000000002</v>
+        <v>0.85714000000000001</v>
       </c>
       <c r="B21" s="1">
-        <v>0.71428999999999998</v>
+        <v>0.85714000000000001</v>
       </c>
       <c r="C21" s="1">
-        <v>0.76190000000000002</v>
+        <v>0.85714000000000001</v>
       </c>
       <c r="D21">
-        <v>0.77778000000000003</v>
+        <v>0.85185</v>
       </c>
       <c r="E21" s="1">
         <v>0.81481000000000003</v>
@@ -5544,34 +5724,34 @@
         <v>0.81481000000000003</v>
       </c>
       <c r="G21">
+        <v>0.77922000000000002</v>
+      </c>
+      <c r="H21">
+        <v>0.74026000000000003</v>
+      </c>
+      <c r="I21">
+        <v>0.74026000000000003</v>
+      </c>
+      <c r="J21">
         <v>0.71428999999999998</v>
       </c>
-      <c r="H21">
-        <v>0.72726999999999997</v>
-      </c>
-      <c r="I21">
-        <v>0.75324999999999998</v>
-      </c>
-      <c r="J21">
-        <v>0.77381</v>
-      </c>
       <c r="K21">
-        <v>0.75</v>
+        <v>0.71428999999999998</v>
       </c>
       <c r="L21">
         <v>0.75</v>
       </c>
       <c r="M21">
-        <v>0.90046999999999999</v>
+        <v>0.91446000000000005</v>
       </c>
       <c r="N21">
-        <v>0.90202000000000004</v>
+        <v>0.90980000000000005</v>
       </c>
       <c r="O21">
-        <v>0.91134999999999999</v>
+        <v>0.90980000000000005</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>0.80952000000000002</v>
       </c>
@@ -5579,111 +5759,111 @@
         <v>0.85714000000000001</v>
       </c>
       <c r="C22" s="1">
-        <v>0.80952000000000002</v>
+        <v>0.76190000000000002</v>
       </c>
       <c r="D22">
         <v>0.88888999999999996</v>
       </c>
       <c r="E22" s="1">
+        <v>0.88888999999999996</v>
+      </c>
+      <c r="F22">
         <v>0.92593000000000003</v>
       </c>
-      <c r="F22">
-        <v>0.74073999999999995</v>
-      </c>
       <c r="G22">
-        <v>0.81579000000000002</v>
+        <v>0.73684000000000005</v>
       </c>
       <c r="H22">
-        <v>0.78947000000000001</v>
+        <v>0.75</v>
       </c>
       <c r="I22">
-        <v>0.78947000000000001</v>
+        <v>0.72367999999999999</v>
       </c>
       <c r="J22">
-        <v>0.78571000000000002</v>
+        <v>0.76190000000000002</v>
       </c>
       <c r="K22">
-        <v>0.78571000000000002</v>
+        <v>0.75</v>
       </c>
       <c r="L22">
-        <v>0.79762</v>
+        <v>0.72619</v>
       </c>
       <c r="M22">
-        <v>0.90046999999999999</v>
+        <v>0.91446000000000005</v>
       </c>
       <c r="N22">
-        <v>0.89736000000000005</v>
+        <v>0.90824000000000005</v>
       </c>
       <c r="O22">
-        <v>0.91601999999999995</v>
+        <v>0.90512999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <f>AVERAGE(A3:A22) * 100</f>
-        <v>74.339750000000009</v>
+        <v>77.835399999999993</v>
       </c>
       <c r="B23">
         <f t="shared" ref="B23:O23" si="0">AVERAGE(B3:B22) * 100</f>
-        <v>75.053999999999988</v>
+        <v>78.755249999999975</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>77.153500000000008</v>
+        <v>78.95004999999999</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>83.703649999999996</v>
+        <v>80.555449999999979</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>82.036850000000001</v>
+        <v>81.296149999999983</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>82.222049999999996</v>
+        <v>81.296149999999983</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>75.721900000000005</v>
+        <v>76.364500000000007</v>
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
-        <v>75.265699999999995</v>
+        <v>75.977399999999989</v>
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>75.008499999999984</v>
+        <v>75.001750000000001</v>
       </c>
       <c r="J23">
         <f t="shared" si="0"/>
-        <v>74.946150000000003</v>
+        <v>74.000749999999996</v>
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>74.76755</v>
+        <v>73.524549999999991</v>
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
-        <v>74.831250000000011</v>
+        <v>74.597400000000007</v>
       </c>
       <c r="M23">
         <f t="shared" si="0"/>
-        <v>91.359750000000005</v>
+        <v>91.305249999999987</v>
       </c>
       <c r="N23">
         <f t="shared" si="0"/>
-        <v>90.87769999999999</v>
+        <v>91.010050000000007</v>
       </c>
       <c r="O23">
         <f t="shared" si="0"/>
-        <v>91.507049999999992</v>
+        <v>91.072149999999993</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>